<commit_message>
Data Update 17 02 25
Trained the model on further questions from a set of questions about GEO tabular data structures.
</commit_message>
<xml_diff>
--- a/query_responses.xlsx
+++ b/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="45" customWidth="1" min="1" max="1"/>
-    <col width="296" customWidth="1" min="2" max="2"/>
+    <col width="871" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -509,6 +509,89 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>how do i edit the table length/width</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>To edit the table length or width, you need to select the cell and then use the "Auto Fit" option. However, this is not explicitly mentioned in the provided documentation.
+A more accurate answer based on the available information would be:
+Unfortunately, the provided documentation does not mention how to directly edit the table length or width.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>how to remove/add columns/rows</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>To delete rows, select the row and press Delete on your keyboard. Note that empty rows (no data) will be treated as valid data points.
+To add or remove columns, follow these steps:
+1. Select the table from the "Select Definition" box in the GEO Home tab.
+2. Click "Load Rows From" and then "Clipboard".
+3. Copy the desired column data from another source (e.g., Microsoft Excel).
+4. In the "Table Values" dialog box, select the table where you want to apply the new template for the same data set.
+5. Click "Export Rows to Clipboard", then delete the existing rows in the clipboard.
+6. Click "Create" and select a new template from the "Template" box.
+7. Click "Apply".
+8. The newly added or removed columns will be displayed in the table.
+Alternatively, you can also use the "Load Rows From" option with a file or clipboard to add or remove columns.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>how to remove the character limit in tables</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>According to the GEO application documentation, there is no direct option to remove the character limit for individual cells in a table. However, you can create a new table template with more columns or different column labels, and then use that template to enter data.
+Additionally, you can maximize the screen to view the table of contents, which may help you better manage your tables within the ODF file's limits.
+Please note that there is no specific information on removing the character limit for individual cells in a table.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>how to import table data</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>To import table data into GEO, follow these steps:
+1. In the GEO Home tab, select the table from the "Select Definition" box.
+2. If the table has not been created, select "Create Table" from the template and pick a category and select a table template.
+3. Click "Clipboard" in the "Load Rows From" section to import all information from the clipboard into the selected table.
+Alternatively, you can also import data from outside of GEO by:
+1. Highlighting new data in your raw data file (e.g., Microsoft Excel).
+2. Ensuring the columns are in sequence with that of the table in GEO and that the depth values are appropriate.
+3. Copying the data to clipboard.
+4. In the GEO Home tab, selecting the table from the "Select Definition" box.
+5. Clicking "Clipboard" from the "Load Rows From" section and confirming you want to append the rows (not replace existing rows).</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>how to remove a table in a layout</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>To remove a table in a layout, select the free format text and hit Delete on your keyboard. Alternatively, right-click on the free format text and select Delete.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Working Refactored Model 18 02 25
Successfully refactored Ollama model for command prompt operation after reshaping the project layout
Removed redundant functions and imports in offline-app.py.
</commit_message>
<xml_diff>
--- a/query_responses.xlsx
+++ b/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -592,6 +592,18 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>What is 1 + 1?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Embedding 18 02 25
Changed Embedding to a free open source HF alternative
</commit_message>
<xml_diff>
--- a/query_responses.xlsx
+++ b/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -604,6 +604,114 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>What is 1 + 1?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>The answer to the question "What is 1 + 1?" is 2.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>What is 1 + 1?</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>The answer to the question "What is 1 + 1?" is 2.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>What is 1 + 1?</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>What is 1 + 1?</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>What is 1 + 1?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>The answer to the question "What is 1 + 1?" is 2.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>What is 1 + 1?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>What is AI?</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>I don't have any information about "AI" in the provided documents. The GEO application seems to be focused on well log authoring, analysis, and reporting for petroleum geologists and engineers. If you could provide more context or clarify what you mean by "AI", I'll do my best to help.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>What is 1 + 1?</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>What is AI?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>I don't have any information about "AI" in the provided documents. The GEO application seems to be focused on well log authoring, analysis, and reporting for petroleum geologists and engineers. If you could provide more context or clarify what you mean by "AI", I'll do my best to help.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Embedding Methods 18 02 25
Standardized embedding methods with HF methods.
</commit_message>
<xml_diff>
--- a/query_responses.xlsx
+++ b/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +433,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="45" customWidth="1" min="1" max="1"/>
+    <col width="47" customWidth="1" min="1" max="1"/>
     <col width="871" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
@@ -712,6 +712,70 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>What are the formats for loading a text file?</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Yes, GEO can load several different types of ASCII files, including tab-delimited and space-delimited files. In addition to these files, also csv (comma-separated value) files can be loaded.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>What is an ODT?</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>An ODT (OpenDocument Template) is a file format used in the GEO application that remains unchanged after generating an ODF (OpenDocument File) from a template, allowing users to reuse it for subsequent wells.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>What is an ODT?</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>An ODT (OpenDocument Template) is a file format used in the GEO application that remains unchanged after generating an ODF (OpenDocument File) from a template, allowing users to reuse it for subsequent wells.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>What is the limit on the number of curves?</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>The limit on the number of curves is 450, with an additional note that the infinite wrapping is limited by the "Maximum number of times to Wrap a Curve" in the Global Settings.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Where can you view the mouse pointer depth?</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>To view the mouse pointer depth, follow these steps:
+1. Go to the Depth tab and select Index Converter or press + on your keyboard.
+2. In the Convert Index dialog box, enter the desired depth or time of the section of log you wish to view.
+3. Click "Go" to instantly display the relevant depth section.
+Alternatively, you can also access this dialog box by going to Tools and selecting Index Converter or using the Mouse &amp; Keyboard Modestoolbar.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>